<commit_message>
fix the bug in FinalProject and Phase3
</commit_message>
<xml_diff>
--- a/payroll.xlsx
+++ b/payroll.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lowyi\OneDrive\Documents\TP\INAUTO\AIPayrollReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFD9803-4A1F-4C1E-BD71-CAB01EE1ABFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BE7AC7-55D4-4B1E-A7F1-6B52B2D48C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5760" yWindow="792" windowWidth="17280" windowHeight="9960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021Mar" sheetId="2" r:id="rId1"/>
     <sheet name="2020Mar" sheetId="5" r:id="rId2"/>
     <sheet name="2019Mar" sheetId="7" r:id="rId3"/>
     <sheet name="2018Mar" sheetId="8" r:id="rId4"/>
-    <sheet name="2021Data" sheetId="9" r:id="rId5"/>
+    <sheet name="I" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="36" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -35,10 +35,10 @@
     <t>LegalStatus</t>
   </si>
   <si>
-    <t>Gender</t>
+    <t>Nationality</t>
   </si>
   <si>
-    <t>Race</t>
+    <t>Gender</t>
   </si>
   <si>
     <t>JobTitle</t>
@@ -542,7 +542,7 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Count of Gender</t>
+    <t>Count of Nationality</t>
   </si>
 </sst>
 </file>
@@ -577,12 +577,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,13 +601,237 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[payroll.xlsx]I!Nationality</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>I!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>I!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>CHINESE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FILIPINO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INDIAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>INDONESIAN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MALAYSIAN</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MYANMAR</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>SINGAPOREAN</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SRI LANKAN</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>VIETNAMESE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>I!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5BF7-4345-9D37-14C9A1D60BA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>543560</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>86360</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C11C4865-44F2-DE62-4156-9886C2E45BAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jun Low" refreshedDate="44929.436337615742" createdVersion="1" refreshedVersion="8" recordCount="101" xr:uid="{A82E30DA-88FC-44B6-A4A7-92D1E8E40DEC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jun Low" refreshedDate="44929.739464699072" createdVersion="1" refreshedVersion="8" recordCount="100" xr:uid="{2ECCD5E0-1E20-4227-9C4A-6A49980114EB}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C1:C102" sheet="2021Mar"/>
+    <worksheetSource ref="C1:C101" sheet="2021Mar"/>
   </cacheSource>
   <cacheFields count="1">
-    <cacheField name="Gender" numFmtId="0">
+    <cacheField name="Nationality" numFmtId="0">
       <sharedItems count="9">
         <s v="SINGAPOREAN"/>
         <s v="VIETNAMESE"/>
@@ -629,7 +854,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="101">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="100">
   <r>
     <x v="0"/>
   </r>
@@ -930,14 +1155,11 @@
   <r>
     <x v="0"/>
   </r>
-  <r>
-    <x v="2"/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{015BFABD-377E-4B9B-8B9E-0812223FD856}" name="Nationality" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B2AD67AC-C5CC-4F73-868A-AF1DAC302A29}" name="Nationality" cacheId="36" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
   <location ref="A1:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0" includeNewItemsInFilter="1">
@@ -999,7 +1221,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of Gender" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of Nationality" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="0" series="1">
@@ -1312,7 +1534,7 @@
   <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C102" sqref="C2:C102"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21162,7 +21384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8385903-2157-451A-91C4-3BDA82E5E04C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E64C564-143B-4CAD-B05E-499CA75EA856}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -21172,7 +21394,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -21187,7 +21409,7 @@
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -21195,7 +21417,7 @@
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>6</v>
       </c>
     </row>
@@ -21203,7 +21425,7 @@
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>30</v>
       </c>
     </row>
@@ -21211,7 +21433,7 @@
       <c r="A5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
     </row>
@@ -21219,7 +21441,7 @@
       <c r="A6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>7</v>
       </c>
     </row>
@@ -21227,15 +21449,15 @@
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B7">
-        <v>34</v>
+      <c r="B7" s="3">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>16</v>
       </c>
     </row>
@@ -21243,7 +21465,7 @@
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>5</v>
       </c>
     </row>
@@ -21251,7 +21473,7 @@
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>1</v>
       </c>
     </row>
@@ -21259,11 +21481,12 @@
       <c r="A11" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B11">
-        <v>101</v>
+      <c r="B11" s="3">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Save chart as picture/completed plotting all chart
</commit_message>
<xml_diff>
--- a/payroll.xlsx
+++ b/payroll.xlsx
@@ -5,29 +5,29 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lowyi\OneDrive\Documents\TP\INAUTO\AIPayrollReport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parod\OneDrive\Documents\UiPath\AiPayRoll2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BE7AC7-55D4-4B1E-A7F1-6B52B2D48C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB1237D-3313-4594-A1B1-2E5117BA63B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5760" yWindow="792" windowWidth="17280" windowHeight="9960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2021Mar" sheetId="2" r:id="rId1"/>
-    <sheet name="2020Mar" sheetId="5" r:id="rId2"/>
-    <sheet name="2019Mar" sheetId="7" r:id="rId3"/>
-    <sheet name="2018Mar" sheetId="8" r:id="rId4"/>
-    <sheet name="I" sheetId="9" r:id="rId5"/>
+    <sheet name="2021MarVl" sheetId="25" r:id="rId1"/>
+    <sheet name="2021Mar" sheetId="2" r:id="rId2"/>
+    <sheet name="2020Mar" sheetId="5" r:id="rId3"/>
+    <sheet name="2019Mar" sheetId="7" r:id="rId4"/>
+    <sheet name="2018Mar" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="36" r:id="rId6"/>
+    <pivotCache cacheId="20" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2428" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2418" uniqueCount="171">
   <si>
     <t>Name</t>
   </si>
@@ -536,13 +536,10 @@
     <t>Myo, Min Htike</t>
   </si>
   <si>
-    <t>Row Labels</t>
+    <t>Sum of CPF_Employee</t>
   </si>
   <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Count of Nationality</t>
+    <t>Sum of CPF_Employer</t>
   </si>
 </sst>
 </file>
@@ -577,12 +574,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -615,7 +608,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[payroll.xlsx]I!Nationality</c:name>
+    <c:name>[payroll.xlsx]2021MarVl!CPF contributions</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -637,17 +630,44 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>I!$B$1</c:f>
+              <c:f>'2021MarVl'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of CPF_Employee</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2021MarVl'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -655,81 +675,66 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2021MarVl'!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>27214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D379-4B40-AD48-2032F0CB3E05}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2021MarVl'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of CPF_Employer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>I!$A$2:$A$11</c:f>
+              <c:f>'2021MarVl'!$A$2</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CHINESE</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>FILIPINO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>INDIAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>INDONESIAN</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>MALAYSIAN</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>MYANMAR</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>SINGAPOREAN</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>SRI LANKAN</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>VIETNAMESE</c:v>
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>I!$B$2:$B$11</c:f>
+              <c:f>'2021MarVl'!$B$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>24760</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5BF7-4345-9D37-14C9A1D60BA0}"/>
+              <c16:uniqueId val="{00000001-D379-4B40-AD48-2032F0CB3E05}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -740,10 +745,45 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="988964527"/>
+        <c:axId val="988965359"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="988964527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="988965359"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="988965359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="988964527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -788,23 +828,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>543560</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>566420</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>86360</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>109220</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Chart 13">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C11C4865-44F2-DE62-4156-9886C2E45BAD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09D2E5AF-8A99-38C2-09DC-0BABBDA62C3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -826,23 +866,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jun Low" refreshedDate="44929.739464699072" createdVersion="1" refreshedVersion="8" recordCount="100" xr:uid="{2ECCD5E0-1E20-4227-9C4A-6A49980114EB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jeff Ong" refreshedDate="44936.745946875002" createdVersion="1" refreshedVersion="8" recordCount="100" xr:uid="{C57FA3F2-FDD4-48CB-86D6-3244EEA7EE65}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C1:C101" sheet="2021Mar"/>
+    <worksheetSource ref="L1:M101" sheet="2021Mar"/>
   </cacheSource>
-  <cacheFields count="1">
-    <cacheField name="Nationality" numFmtId="0">
-      <sharedItems count="9">
-        <s v="SINGAPOREAN"/>
-        <s v="VIETNAMESE"/>
-        <s v="MYANMAR"/>
-        <s v="FILIPINO"/>
-        <s v="SRI LANKAN"/>
-        <s v="INDIAN"/>
-        <s v="MALAYSIAN"/>
-        <s v="INDONESIAN"/>
-        <s v="CHINESE"/>
-      </sharedItems>
+  <cacheFields count="2">
+    <cacheField name="CPF_Employee" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1200"/>
+    </cacheField>
+    <cacheField name="CPF_Employer" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1020"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -856,325 +889,420 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="100">
   <r>
-    <x v="0"/>
+    <n v="780"/>
+    <n v="780"/>
   </r>
   <r>
-    <x v="1"/>
+    <n v="1000"/>
+    <n v="850"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="780"/>
+    <n v="780"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="3"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="510"/>
+    <n v="434"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="230"/>
+    <n v="345"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="940"/>
+    <n v="799"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="1020"/>
+    <n v="867"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="367"/>
+    <n v="442"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="250"/>
+    <n v="375"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="3"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="6"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="1160"/>
+    <n v="986"/>
   </r>
   <r>
-    <x v="7"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="4"/>
+    <n v="1140"/>
+    <n v="969"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="780"/>
+    <n v="780"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="650"/>
+    <n v="650"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="3"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="6"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="225"/>
+    <n v="338"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="650"/>
+    <n v="650"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="240"/>
+    <n v="360"/>
   </r>
   <r>
-    <x v="3"/>
+    <n v="650"/>
+    <n v="650"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="1200"/>
+    <n v="1020"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="300"/>
+    <n v="360"/>
   </r>
   <r>
-    <x v="8"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="6"/>
+    <n v="700"/>
+    <n v="595"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="162"/>
+    <n v="244"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="6"/>
+    <n v="280"/>
+    <n v="238"/>
   </r>
   <r>
-    <x v="3"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="3"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="300"/>
+    <n v="255"/>
   </r>
   <r>
-    <x v="6"/>
+    <n v="182"/>
+    <n v="182"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="5"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
-    <x v="6"/>
+    <n v="682"/>
+    <n v="580"/>
   </r>
   <r>
-    <x v="6"/>
+    <n v="400"/>
+    <n v="340"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="300"/>
+    <n v="255"/>
   </r>
   <r>
-    <x v="2"/>
+    <n v="1100"/>
+    <n v="935"/>
   </r>
   <r>
-    <x v="0"/>
+    <n v="636"/>
+    <n v="541"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B2AD67AC-C5CC-4F73-868A-AF1DAC302A29}" name="Nationality" cacheId="36" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
-  <location ref="A1:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" showAll="0" includeNewItemsInFilter="1">
-      <items count="10">
-        <item x="8"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3EFAA8BB-C23B-43BB-884E-CAD7CEB3CFDF}" name="CPF contributions" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" pageOverThenDown="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
+  <location ref="A1:B2" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
@@ -1182,53 +1310,39 @@
       </extLst>
     </pivotField>
   </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="10">
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
     <i>
       <x/>
     </i>
-    <i>
+    <i i="1">
       <x v="1"/>
     </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Nationality" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  <dataFields count="2">
+    <dataField name="Sum of CPF_Employee" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Sum of CPF_Employer" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -1530,11 +1644,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE76A62-56C5-4336-BE97-616BF2172F2F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>27214</v>
+      </c>
+      <c r="B2" s="1">
+        <v>24760</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6644,7 +6792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P112"/>
   <sheetViews>
@@ -12257,11 +12405,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A74" zoomScale="94" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:J101"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -17370,7 +17520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P80"/>
   <sheetViews>
@@ -21381,112 +21531,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E64C564-143B-4CAD-B05E-499CA75EA856}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="3">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>